<commit_message>
Finalizando mudanças na branch atualizacao-tabelas-e-menus
</commit_message>
<xml_diff>
--- a/input/projetos.xlsx
+++ b/input/projetos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\OneDrive\Área de Trabalho\python-whatsapp\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\OneDrive\Área de Trabalho\python-whatsapp\chatbot\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FA46EC-879E-44A0-8F41-7D174DF26F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD690248-CEC7-4930-9CC2-74B1CE88513A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{892F52A2-84FF-4991-B4B4-2F3F5E24F9F0}"/>
   </bookViews>
@@ -25,51 +25,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
   <si>
     <t>id_projeto</t>
   </si>
   <si>
-    <t>id_tipo_produto</t>
+    <t>medida_final</t>
+  </si>
+  <si>
+    <t>FIXO</t>
+  </si>
+  <si>
+    <t>id_formula</t>
+  </si>
+  <si>
+    <t>definicao_1</t>
+  </si>
+  <si>
+    <t>definicao_2</t>
+  </si>
+  <si>
+    <t>definicao_3</t>
+  </si>
+  <si>
+    <t>FECHADURA 3530</t>
+  </si>
+  <si>
+    <t>JANELA DE ABRIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHADURA 3530 E PUXADOR H </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUXADOR H </t>
+  </si>
+  <si>
+    <t>4 FOLHAS</t>
+  </si>
+  <si>
+    <t>2 FOLHAS</t>
+  </si>
+  <si>
+    <t>PORTA DE ABRIR</t>
+  </si>
+  <si>
+    <t>BASCULANTE</t>
+  </si>
+  <si>
+    <t>PEQUENO (FERRAGEM PEQ)</t>
+  </si>
+  <si>
+    <t>GRANDE (ORELHA MICKEY)</t>
   </si>
   <si>
     <t>descricao_projeto</t>
   </si>
   <si>
-    <t>medida_final</t>
-  </si>
-  <si>
-    <t>FIXO</t>
-  </si>
-  <si>
-    <t>id_formula</t>
-  </si>
-  <si>
-    <t>JANELA DE ABRIR COM FECHADURA 3530</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JANELA DE ABRIR COM FECHADURA 3530 E PUXADOR H </t>
-  </si>
-  <si>
-    <t>JANELA DE ABRIR COM PUXADOR H</t>
-  </si>
-  <si>
-    <t>JANELA DE ABRIR DE 4 FOLHAS COM PUXADOR H</t>
-  </si>
-  <si>
-    <t>JANELA DE ABRIR DE 4 FOLHAS COM FECHADURA 3530</t>
-  </si>
-  <si>
-    <t>JANELA DE ABRIR DE 4 FOLHAS COM FECHADURA 3530 E PUXADOR H</t>
-  </si>
-  <si>
-    <t>JANELA DE ABRIR DE 2 FOLHAS COM PUXADOR H</t>
-  </si>
-  <si>
-    <t>JANELA DE ABRIR DE 2 FOLHAS COM FECHADURA 3530</t>
-  </si>
-  <si>
-    <t>JANELA DE ABRIR DE 2 FOLHAS COM FECHADURA 3530 E PUXADOR H</t>
+    <t>FIXO - MEDIDA FINAL</t>
+  </si>
+  <si>
+    <t>FIXO - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>JANELA DE ABRIR - FECHADURA 3530 E PUXADOR H - MEDIDA FINAL</t>
+  </si>
+  <si>
+    <t>JANELA DE ABRIR - PUXADOR H - MEDIDA FINAL</t>
+  </si>
+  <si>
+    <t>JANELA DE ABRIR - FECHADURA 3530 - MEDIDA FINAL</t>
+  </si>
+  <si>
+    <t>PORTA DE ABRIR - FECHADURA 3530 - MEDIDA FINAL</t>
+  </si>
+  <si>
+    <t>PORTA DE ABRIR - PUXADOR H - MEDIDA FINAL</t>
+  </si>
+  <si>
+    <t>PORTA DE ABRIR - FECHADURA 3530 E PUXADOR H - MEDIDA FINAL</t>
+  </si>
+  <si>
+    <t>JANELA DE ABRIR - 4 FOLHAS - FECHADURA 3530 E PUXADOR H - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>JANELA DE ABRIR - 2 FOLHAS - FECHADURA 3530 - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>JANELA DE ABRIR - 2 FOLHAS - PUXADOR H - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>JANELA DE ABRIR - 2 FOLHAS - FECHADURA 3530 E PUXADOR H - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>PORTA DE ABRIR - 4 FOLHAS - FECHADURA 3530 - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>PORTA DE ABRIR - 4 FOLHAS - PUXADOR H - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>PORTA DE ABRIR - 4 FOLHAS - FECHADURA 3530 E PUXADOR H - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>PORTA DE ABRIR - 2 FOLHAS - FECHADURA 3530 - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>PORTA DE ABRIR - 2 FOLHAS - PUXADOR H - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>PORTA DE ABRIR - 2 FOLHAS - FECHADURA 3530 E PUXADOR H - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>JANELA DE ABRIR - 4 FOLHAS - PUXADOR H - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>JANELA DE ABRIR - 4 FOLHAS - FECHADURA 3530 - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>BASCULANTE - PEQUENO - MEDIDA FINAL</t>
+  </si>
+  <si>
+    <t>BASCULANTE - GRANDE - MEDIDA FINAL</t>
+  </si>
+  <si>
+    <t>BASCULANTE - PEQUENO - MEDIDA VÃO</t>
+  </si>
+  <si>
+    <t>BASCULANTE - GRANDE - MEDIDA VÃO</t>
   </si>
 </sst>
 </file>
@@ -421,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609BBFCD-F251-4F6E-AC6D-4EEF90371259}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G25" sqref="A1:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,11 +513,12 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,200 +526,529 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
         <v>14</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>